<commit_message>
All steps up to dictionary creation
</commit_message>
<xml_diff>
--- a/HDR23-24_Statistical_Annex_PHDI_Table.xlsx
+++ b/HDR23-24_Statistical_Annex_PHDI_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admir.jahic\Desktop\HDR 2023-24\Final files for launch\Final files for launch\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ydubey/Desktop/planetaryhdi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56D73B68-895E-43F5-B0FC-9103273B79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B68FDEA-5A82-4F44-823E-692D5F18508F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3AF1E20E-4309-4781-9DFA-6736AE4D1C5A}"/>
+    <workbookView xWindow="7500" yWindow="1180" windowWidth="33240" windowHeight="19380" xr2:uid="{3AF1E20E-4309-4781-9DFA-6736AE4D1C5A}"/>
   </bookViews>
   <sheets>
     <sheet name="PHDI" sheetId="4" r:id="rId1"/>
@@ -1573,47 +1573,47 @@
   <dimension ref="A1:AH257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="J218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C235" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K227" sqref="K227"/>
+      <selection pane="bottomRight" activeCell="B238" sqref="B238:AC238"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.73046875" style="1"/>
-    <col min="2" max="2" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="91" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.86328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.59765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.59765625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="2" style="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.73046875" style="1"/>
+    <col min="22" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:20" s="5" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:20" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:20" s="5" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:20" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="M5" s="7" t="s">
         <v>226</v>
       </c>
@@ -1621,8 +1621,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:20" s="8" customFormat="1" ht="69.400000000000006" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:20" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" s="8" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" s="8" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="T8" s="9"/>
     </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="C9" s="18">
         <v>2022</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>202</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="S10" s="20"/>
       <c r="T10" s="20"/>
     </row>
-    <row r="11" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="21">
         <v>1</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>0.76145930975713683</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="21">
         <v>2</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>0.7723938361028263</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="21">
         <v>3</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>0.80509231643232493</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="21">
         <v>4</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="21">
         <v>5</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>0.8279164891350661</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="21">
         <v>5</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>0.81054324669791222</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="21">
         <v>7</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0.85894333191308048</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="21">
         <v>7</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>0.81290512711262608</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="21">
         <v>9</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0.69357477631018316</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="21">
         <v>10</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>0.80880201675898311</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="21">
         <v>10</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>0.78825379917625338</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="21">
         <v>12</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>0.81148771481323678</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="21">
         <v>12</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>0.75950575202386028</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="21">
         <v>12</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="21">
         <v>15</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>0.86755148416418126</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="21">
         <v>16</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0.82109146428064195</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="21">
         <v>17</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>0.80000568101121994</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="21">
         <v>18</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0.73612199971594938</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="21">
         <v>19</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0.82463854566112771</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="21">
         <v>20</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>0.65068669223121711</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="21">
         <v>20</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>0.79157932111915918</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="21">
         <v>22</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>0.80143374520664679</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="21">
         <v>22</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0.87656085783269422</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="21">
         <v>24</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.86889788382332056</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="21">
         <v>25</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>0.78530251384746486</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="21">
         <v>25</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>0.80086848459025717</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="21">
         <v>27</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>0.90570089475926707</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="21">
         <v>28</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>0.87180940207356905</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="21">
         <v>29</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0.84523292146001994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="21">
         <v>30</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>0.89470955830137766</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="21">
         <v>31</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>0.80617880982814938</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="21">
         <v>32</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>0.86804573214032099</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="21">
         <v>33</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>0.88479548359608007</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="21">
         <v>34</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>0.85579960232921459</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="21">
         <v>35</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="21">
         <v>36</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>0.88275316006249116</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="21">
         <v>37</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>0.83029541258343986</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="21">
         <v>37</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0.76689816787388154</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="21">
         <v>39</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0.89514202528049991</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="21">
         <v>40</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0.54842209913364581</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="21">
         <v>40</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>0.80754296264735126</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="21">
         <v>42</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>0.89841073711120578</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="21">
         <v>43</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="21">
         <v>44</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>0.88805851441556594</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="21">
         <v>45</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0.89923590399091036</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="21">
         <v>45</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>0.90176608436301664</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="21">
         <v>47</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>0.87299531316574353</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="21">
         <v>48</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>0.89737821332197132</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="21">
         <v>49</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>0.68788950433177098</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="21">
         <v>50</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="21">
         <v>51</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="21">
         <v>52</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>0.92071154665530464</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="21">
         <v>53</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>0.88667305780428918</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="21">
         <v>54</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="21">
         <v>55</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>0.73136841357761684</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="21">
         <v>56</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>0.91939355205226525</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="21">
         <v>57</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>0.88161269706007672</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="21">
         <v>57</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>0.92107371112057956</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="21">
         <v>59</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>0.65232282346257631</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="21">
         <v>60</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>0.92236614117312876</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="21">
         <v>60</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A72" s="21">
         <v>62</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="21">
         <v>63</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0.85197060076693654</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="21">
         <v>64</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>0.91311177389575338</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="21">
         <v>65</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>0.89732779434739385</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A76" s="21">
         <v>66</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0.91633787814230938</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="21">
         <v>67</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>0.88887942053685554</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="21">
         <v>67</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="21">
         <v>69</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="1:20" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:20" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B80" s="20" t="s">
         <v>204</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="S80" s="20"/>
       <c r="T80" s="20"/>
     </row>
-    <row r="81" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="21">
         <v>70</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>0.88258699048430622</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="21">
         <v>71</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="21">
         <v>72</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A84" s="21">
         <v>73</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A85" s="21">
         <v>74</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>0.91665459451782405</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="21">
         <v>75</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>0.82755858542820626</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="21">
         <v>76</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>0.94776807271694363</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="21">
         <v>77</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>0.92695284760687413</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="21">
         <v>78</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>0.93671992614685406</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A90" s="21">
         <v>78</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>0.96467618236046015</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="21">
         <v>80</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>0.90130947308620935</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="21">
         <v>81</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="21">
         <v>82</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>0.93994603039341007</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="21">
         <v>83</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>0.94506746200823744</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="21">
         <v>83</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>0.91741087913648622</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A96" s="21">
         <v>85</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0.96028831131941494</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="21">
         <v>86</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>0.9394503621644652</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="21">
         <v>87</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A99" s="21">
         <v>87</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>0.94486507598352498</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="21">
         <v>89</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>0.94078610992756706</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="21">
         <v>89</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>0.87858613833262322</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="21">
         <v>91</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>0.93735761965629871</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="21">
         <v>92</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>0.89622567817071441</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="21">
         <v>93</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>0.93807768782843348</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="21">
         <v>94</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>0.92417554324669782</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="21">
         <v>95</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="21">
         <v>96</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>0.82029541258343985</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="21">
         <v>97</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="21">
         <v>98</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A110" s="21">
         <v>99</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>0.94634071864791935</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="21">
         <v>100</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>0.93049282772333464</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A112" s="21">
         <v>101</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>0.95226530322397385</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A113" s="21">
         <v>102</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A114" s="21">
         <v>102</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>0.89073640107939211</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="21">
         <v>104</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="21">
         <v>105</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>0.94000710126402509</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="21">
         <v>106</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0.96008592529470249</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A118" s="21">
         <v>107</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>0.92358045732140315</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A119" s="21">
         <v>108</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A120" s="21">
         <v>109</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>0.93468328362448516</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A121" s="21">
         <v>110</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>0.95272759551200104</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A122" s="21">
         <v>111</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>0.9492628887942054</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A123" s="21">
         <v>112</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>0.95015267717653751</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A124" s="21">
         <v>113</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>0.9520245703735265</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A125" s="21">
         <v>114</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>0.94341428774321823</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A126" s="21">
         <v>115</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>0.94522155943757991</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A127" s="21">
         <v>116</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A128" s="21">
         <v>117</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>0.96848601050987071</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A129" s="21">
         <v>118</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>0.93058514415565963</v>
       </c>
     </row>
-    <row r="130" spans="1:20" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:20" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B130" s="20" t="s">
         <v>205</v>
       </c>
@@ -5933,7 +5933,7 @@
       <c r="S130" s="20"/>
       <c r="T130" s="20"/>
     </row>
-    <row r="131" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A131" s="21">
         <v>119</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>0.93358826871183065</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A132" s="21">
         <v>120</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>0.91961653174265012</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A133" s="21">
         <v>120</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>0.9516851299531317</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A134" s="21">
         <v>122</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A135" s="21">
         <v>123</v>
       </c>
@@ -6108,7 +6108,7 @@
         <v>0.95805851441556589</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A136" s="21">
         <v>124</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A137" s="21">
         <v>125</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>0.82431614827439281</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A138" s="21">
         <v>126</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>0.96867774463854572</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A139" s="21">
         <v>127</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>0.94158003124556178</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A140" s="21">
         <v>128</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>0.96288098281494106</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A141" s="21">
         <v>129</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>0.96700965771907399</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A142" s="21">
         <v>130</v>
       </c>
@@ -6353,7 +6353,7 @@
         <v>0.92922738247408032</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A143" s="21">
         <v>131</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A144" s="21">
         <v>132</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A145" s="21">
         <v>133</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>0.96446385456611283</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A146" s="21">
         <v>134</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>0.96602684277801454</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A147" s="21">
         <v>135</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A148" s="21">
         <v>136</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>0.93523931259764248</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A149" s="21">
         <v>137</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A150" s="21">
         <v>138</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>0.95683993750887664</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A151" s="21">
         <v>139</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>0.91360034086067321</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A152" s="21">
         <v>140</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A153" s="21">
         <v>141</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A154" s="21">
         <v>142</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A155" s="21">
         <v>142</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>0.93500355063201235</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A156" s="21">
         <v>144</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>0.96789873597500353</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A157" s="21">
         <v>145</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>0.95676466411021155</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A158" s="21">
         <v>146</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>0.96907754580315297</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A159" s="21">
         <v>146</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>0.93997443544950998</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A160" s="21">
         <v>148</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>0.92259906263314873</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A161" s="21">
         <v>149</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>0.97369478767220574</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A162" s="21">
         <v>150</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>0.97403209771339294</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A163" s="21">
         <v>151</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>0.97159494390001422</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A164" s="21">
         <v>152</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A165" s="21">
         <v>153</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>0.97892628887942046</v>
       </c>
     </row>
-    <row r="166" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A166" s="21">
         <v>154</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>0.97572219855134212</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A167" s="21">
         <v>155</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A168" s="21">
         <v>156</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A169" s="21">
         <v>157</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A170" s="21">
         <v>158</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>0.98094659849453203</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A171" s="21">
         <v>159</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>0.9766872603323391</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A172" s="21">
         <v>159</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>0.9734213890072434</v>
       </c>
     </row>
-    <row r="173" spans="1:22" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:22" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B173" s="20" t="s">
         <v>206</v>
       </c>
@@ -7426,7 +7426,7 @@
       <c r="S173" s="20"/>
       <c r="T173" s="20"/>
     </row>
-    <row r="174" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A174" s="21">
         <v>161</v>
       </c>
@@ -7463,7 +7463,7 @@
       <c r="U174" s="21"/>
       <c r="V174" s="26"/>
     </row>
-    <row r="175" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A175" s="21">
         <v>161</v>
       </c>
@@ -7500,7 +7500,7 @@
       <c r="U175" s="21"/>
       <c r="V175" s="26"/>
     </row>
-    <row r="176" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A176" s="21">
         <v>163</v>
       </c>
@@ -7537,7 +7537,7 @@
       <c r="U176" s="21"/>
       <c r="V176" s="26"/>
     </row>
-    <row r="177" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A177" s="21">
         <v>164</v>
       </c>
@@ -7574,7 +7574,7 @@
       <c r="U177" s="21"/>
       <c r="V177" s="26"/>
     </row>
-    <row r="178" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A178" s="21">
         <v>164</v>
       </c>
@@ -7611,7 +7611,7 @@
       <c r="U178" s="21"/>
       <c r="V178" s="26"/>
     </row>
-    <row r="179" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A179" s="21">
         <v>166</v>
       </c>
@@ -7648,7 +7648,7 @@
       <c r="U179" s="25"/>
       <c r="V179" s="26"/>
     </row>
-    <row r="180" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A180" s="21">
         <v>167</v>
       </c>
@@ -7685,7 +7685,7 @@
       <c r="U180" s="21"/>
       <c r="V180" s="26"/>
     </row>
-    <row r="181" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A181" s="21">
         <v>168</v>
       </c>
@@ -7722,7 +7722,7 @@
       <c r="U181" s="25"/>
       <c r="V181" s="26"/>
     </row>
-    <row r="182" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A182" s="21">
         <v>169</v>
       </c>
@@ -7759,7 +7759,7 @@
       <c r="U182" s="21"/>
       <c r="V182" s="26"/>
     </row>
-    <row r="183" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A183" s="21">
         <v>170</v>
       </c>
@@ -7796,7 +7796,7 @@
       <c r="U183" s="21"/>
       <c r="V183" s="26"/>
     </row>
-    <row r="184" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A184" s="21">
         <v>171</v>
       </c>
@@ -7833,7 +7833,7 @@
       <c r="U184" s="21"/>
       <c r="V184" s="26"/>
     </row>
-    <row r="185" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A185" s="21">
         <v>172</v>
       </c>
@@ -7870,7 +7870,7 @@
       <c r="U185" s="21"/>
       <c r="V185" s="26"/>
     </row>
-    <row r="186" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A186" s="21">
         <v>173</v>
       </c>
@@ -7907,7 +7907,7 @@
       <c r="U186" s="21"/>
       <c r="V186" s="26"/>
     </row>
-    <row r="187" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A187" s="21">
         <v>174</v>
       </c>
@@ -7944,7 +7944,7 @@
       <c r="U187" s="21"/>
       <c r="V187" s="26"/>
     </row>
-    <row r="188" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A188" s="21">
         <v>175</v>
       </c>
@@ -7981,7 +7981,7 @@
       <c r="U188" s="21"/>
       <c r="V188" s="26"/>
     </row>
-    <row r="189" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A189" s="21">
         <v>176</v>
       </c>
@@ -8018,7 +8018,7 @@
       <c r="U189" s="21"/>
       <c r="V189" s="26"/>
     </row>
-    <row r="190" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A190" s="21">
         <v>177</v>
       </c>
@@ -8055,7 +8055,7 @@
       <c r="U190" s="21"/>
       <c r="V190" s="26"/>
     </row>
-    <row r="191" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A191" s="21">
         <v>177</v>
       </c>
@@ -8092,7 +8092,7 @@
       <c r="U191" s="21"/>
       <c r="V191" s="26"/>
     </row>
-    <row r="192" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A192" s="21">
         <v>179</v>
       </c>
@@ -8129,7 +8129,7 @@
       <c r="U192" s="25"/>
       <c r="V192" s="26"/>
     </row>
-    <row r="193" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A193" s="21">
         <v>180</v>
       </c>
@@ -8166,7 +8166,7 @@
       <c r="U193" s="21"/>
       <c r="V193" s="26"/>
     </row>
-    <row r="194" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A194" s="21">
         <v>181</v>
       </c>
@@ -8203,7 +8203,7 @@
       <c r="U194" s="21"/>
       <c r="V194" s="26"/>
     </row>
-    <row r="195" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A195" s="21">
         <v>182</v>
       </c>
@@ -8240,7 +8240,7 @@
       <c r="U195" s="21"/>
       <c r="V195" s="26"/>
     </row>
-    <row r="196" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A196" s="21">
         <v>183</v>
       </c>
@@ -8277,7 +8277,7 @@
       <c r="U196" s="21"/>
       <c r="V196" s="26"/>
     </row>
-    <row r="197" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A197" s="21">
         <v>184</v>
       </c>
@@ -8314,7 +8314,7 @@
       <c r="U197" s="21"/>
       <c r="V197" s="26"/>
     </row>
-    <row r="198" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A198" s="21">
         <v>185</v>
       </c>
@@ -8351,7 +8351,7 @@
       <c r="U198" s="21"/>
       <c r="V198" s="26"/>
     </row>
-    <row r="199" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A199" s="21">
         <v>186</v>
       </c>
@@ -8388,7 +8388,7 @@
       <c r="U199" s="21"/>
       <c r="V199" s="26"/>
     </row>
-    <row r="200" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A200" s="21">
         <v>187</v>
       </c>
@@ -8425,7 +8425,7 @@
       <c r="U200" s="21"/>
       <c r="V200" s="26"/>
     </row>
-    <row r="201" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A201" s="21">
         <v>188</v>
       </c>
@@ -8462,7 +8462,7 @@
       <c r="U201" s="21"/>
       <c r="V201" s="26"/>
     </row>
-    <row r="202" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A202" s="21">
         <v>189</v>
       </c>
@@ -8499,7 +8499,7 @@
       <c r="U202" s="21"/>
       <c r="V202" s="26"/>
     </row>
-    <row r="203" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A203" s="21">
         <v>189</v>
       </c>
@@ -8536,7 +8536,7 @@
       <c r="U203" s="21"/>
       <c r="V203" s="26"/>
     </row>
-    <row r="204" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A204" s="21">
         <v>191</v>
       </c>
@@ -8573,7 +8573,7 @@
       <c r="U204" s="21"/>
       <c r="V204" s="26"/>
     </row>
-    <row r="205" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A205" s="21">
         <v>192</v>
       </c>
@@ -8610,7 +8610,7 @@
       <c r="U205" s="21"/>
       <c r="V205" s="26"/>
     </row>
-    <row r="206" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="A206" s="21">
         <v>193</v>
       </c>
@@ -8647,7 +8647,7 @@
       <c r="U206" s="21"/>
       <c r="V206" s="26"/>
     </row>
-    <row r="207" spans="1:22" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:22" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B207" s="20" t="s">
         <v>222</v>
       </c>
@@ -8670,7 +8670,7 @@
       <c r="S207" s="20"/>
       <c r="T207" s="20"/>
     </row>
-    <row r="208" spans="1:22" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:22" ht="14" x14ac:dyDescent="0.15">
       <c r="B208" s="22" t="s">
         <v>199</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="209" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B209" s="22" t="s">
         <v>200</v>
       </c>
@@ -8734,8 +8734,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="210" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="211" spans="1:34" s="29" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="211" spans="1:34" s="29" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A211" s="28"/>
       <c r="B211" s="20" t="s">
         <v>201</v>
@@ -8773,7 +8773,7 @@
       <c r="AG211" s="8"/>
       <c r="AH211" s="8"/>
     </row>
-    <row r="212" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B212" s="22" t="s">
         <v>202</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>0.85102365471445829</v>
       </c>
     </row>
-    <row r="213" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B213" s="22" t="s">
         <v>204</v>
       </c>
@@ -8837,7 +8837,7 @@
         <v>0.88029367391151725</v>
       </c>
     </row>
-    <row r="214" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B214" s="22" t="s">
         <v>205</v>
       </c>
@@ -8869,7 +8869,7 @@
         <v>0.96436476733242471</v>
       </c>
     </row>
-    <row r="215" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B215" s="22" t="s">
         <v>206</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>0.97503241935389051</v>
       </c>
     </row>
-    <row r="216" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B216" s="22"/>
       <c r="C216" s="23"/>
       <c r="E216" s="23"/>
@@ -8913,7 +8913,7 @@
       <c r="Q216" s="24"/>
       <c r="S216" s="23"/>
     </row>
-    <row r="217" spans="1:34" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B217" s="30" t="s">
         <v>207</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>0.92439016115316353</v>
       </c>
     </row>
-    <row r="218" spans="1:34" s="27" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:34" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B218" s="6"/>
       <c r="C218" s="31"/>
       <c r="E218" s="32"/>
@@ -8956,7 +8956,7 @@
       <c r="O218" s="34"/>
       <c r="Q218" s="34"/>
     </row>
-    <row r="219" spans="1:34" s="29" customFormat="1" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:34" s="29" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A219" s="28"/>
       <c r="B219" s="20" t="s">
         <v>208</v>
@@ -8993,7 +8993,7 @@
       <c r="AF219" s="8"/>
       <c r="AG219" s="27"/>
     </row>
-    <row r="220" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B220" s="22" t="s">
         <v>209</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>0.9290856234598931</v>
       </c>
     </row>
-    <row r="221" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B221" s="22" t="s">
         <v>210</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>0.86307133770333</v>
       </c>
     </row>
-    <row r="222" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B222" s="22" t="s">
         <v>211</v>
       </c>
@@ -9089,7 +9089,7 @@
         <v>0.92254029795221149</v>
       </c>
     </row>
-    <row r="223" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B223" s="22" t="s">
         <v>212</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>0.91226877057432587</v>
       </c>
     </row>
-    <row r="224" spans="1:34" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B224" s="22" t="s">
         <v>213</v>
       </c>
@@ -9153,7 +9153,7 @@
         <v>0.96532559331915591</v>
       </c>
     </row>
-    <row r="225" spans="2:29" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B225" s="22" t="s">
         <v>214</v>
       </c>
@@ -9185,11 +9185,11 @@
         <v>0.97310767703640288</v>
       </c>
     </row>
-    <row r="226" spans="2:29" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B226" s="22"/>
       <c r="U226" s="4"/>
     </row>
-    <row r="227" spans="2:29" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B227" s="6" t="s">
         <v>215</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>0.97277681164243734</v>
       </c>
     </row>
-    <row r="228" spans="2:29" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B228" s="35" t="s">
         <v>216</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="229" spans="2:29" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B229" s="22"/>
       <c r="C229" s="23"/>
       <c r="E229" s="25"/>
@@ -9265,7 +9265,7 @@
       <c r="Q229" s="25"/>
       <c r="S229" s="25"/>
     </row>
-    <row r="230" spans="2:29" ht="27.75" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:29" ht="30" x14ac:dyDescent="0.15">
       <c r="B230" s="36" t="s">
         <v>217</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>0.85115002886558466</v>
       </c>
     </row>
-    <row r="231" spans="2:29" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B231" s="22"/>
       <c r="C231" s="23"/>
       <c r="E231" s="23"/>
@@ -9309,7 +9309,7 @@
       <c r="Q231" s="24"/>
       <c r="S231" s="23"/>
     </row>
-    <row r="232" spans="2:29" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="232" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B232" s="30" t="s">
         <v>218</v>
       </c>
@@ -9341,22 +9341,22 @@
         <v>0.91144326300287493</v>
       </c>
     </row>
-    <row r="234" spans="2:29" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B234" s="37" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="235" spans="2:29" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:29" ht="14" x14ac:dyDescent="0.15">
       <c r="B235" s="22" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="2:29" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="237" spans="2:29" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B237" s="38" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="238" spans="2:29" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:29" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B238" s="41" t="s">
         <v>237</v>
       </c>
@@ -9388,93 +9388,93 @@
       <c r="AB238" s="42"/>
       <c r="AC238" s="42"/>
     </row>
-    <row r="239" spans="2:29" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="239" spans="2:29" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B239" s="38" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="2:29" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:29" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B240" s="38" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B241" s="38" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="242" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B242" s="38" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="243" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B243" s="38" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B244" s="38" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="245" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B245" s="38" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="2:2" s="8" customFormat="1" ht="13.9" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:2" s="8" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="B246" s="38" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="2:2" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="248" spans="2:2" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="247" spans="2:2" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="248" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B248" s="30" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B249" s="22" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="250" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B250" s="22" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="251" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B251" s="22" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="252" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B252" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="253" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B253" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="254" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B254" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="255" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B255" s="22" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="256" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B256" s="22" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="257" spans="2:2" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B257" s="22" t="s">
         <v>253</v>
       </c>
@@ -9491,6 +9491,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="7f64e6aa-b736-4f26-84cc-faf427629e48">
@@ -9502,15 +9511,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9719,19 +9719,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9A0FC4C-2605-4EE2-82B5-3922C3B005FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B325BC6-7C16-42DD-86CE-D59B3F647B4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="7f64e6aa-b736-4f26-84cc-faf427629e48"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9A0FC4C-2605-4EE2-82B5-3922C3B005FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>